<commit_message>
ready for module 30
</commit_message>
<xml_diff>
--- a/admin/IB_OB_FLD.xlsx
+++ b/admin/IB_OB_FLD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RW\EAISI-Pythia\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RW\EAISI-Pythia\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1465EB9-FAF5-4C82-A8CD-8E8D63C1CAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C193D-FC77-4E4D-AAF2-9A88F1C48693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="-110" windowWidth="37430" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_LOADS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="615">
   <si>
     <t>SYSTID</t>
   </si>
@@ -1867,6 +1867,21 @@
   </si>
   <si>
     <t>ET/pythia/dat</t>
+  </si>
+  <si>
+    <t>REPEAT</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>SELECT 
+  max( /BIC/ASDSFRPR17~/BIC/VERSMON )
+ FROM 
+  /BIC/ASDSFRPR17</t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1960,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1958,6 +1973,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1988,8 +2006,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:O226" totalsRowShown="0">
-  <autoFilter ref="A1:O226" xr:uid="{00000000-0009-0000-0100-000003000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:Q226" totalsRowShown="0">
+  <autoFilter ref="A1:Q226" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="8">
       <filters>
         <filter val="OH_FRPR1"/>
@@ -2010,17 +2028,11 @@
         <filter val="SDSFRPR3_20250X"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="14">
-      <filters>
-        <filter val="Init 2024"/>
-        <filter val="Last Version"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:O226">
     <sortCondition ref="L34:L226"/>
   </sortState>
-  <tableColumns count="15">
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SYSTID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CLIENT"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FILEINTERN"/>
@@ -2036,6 +2048,8 @@
     <tableColumn id="16" xr3:uid="{3B4693E2-EBA5-46B4-97C9-D51B4B0CBF82}" name="DATE"/>
     <tableColumn id="17" xr3:uid="{5F60B4F6-B6FE-4C4A-99FE-84BA73760AC4}" name="S1B -&gt; S2S"/>
     <tableColumn id="18" xr3:uid="{F55B9E97-2B13-448C-B575-C4B0834B5962}" name="Column1"/>
+    <tableColumn id="12" xr3:uid="{1CB3EDD4-A8FA-46CF-AA4F-81B2540CF816}" name="REPEAT"/>
+    <tableColumn id="13" xr3:uid="{03A11749-D3F7-4D01-A89C-2C1F0AB0E80A}" name="SQL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2045,8 +2059,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C087D875-1D81-4B7D-AAD3-C8B87BB4BDB3}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0">
   <autoFilter ref="A1:E18" xr:uid="{C087D875-1D81-4B7D-AAD3-C8B87BB4BDB3}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{C4C8CC9A-DFD0-4917-B03A-6C233D59BD9C}" name="SUB" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{1204FBB4-A7FE-4F81-9946-60FB97302759}" name="VAR" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{C4C8CC9A-DFD0-4917-B03A-6C233D59BD9C}" name="SUB" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1204FBB4-A7FE-4F81-9946-60FB97302759}" name="VAR" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{5C8E7DB8-E281-4857-8059-8B8D87C650E1}" name="VALUE"/>
     <tableColumn id="3" xr3:uid="{E7C24960-E865-4339-94A3-C4BF4987FB11}" name="SELECT"/>
     <tableColumn id="4" xr3:uid="{98BA64D9-F774-47D3-960D-720A2B56AC5A}" name="Comment"/>
@@ -2334,29 +2348,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O226"/>
+  <dimension ref="A1:Q226"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G265" sqref="G265"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L232" sqref="L232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" customWidth="1"/>
+    <col min="8" max="8" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" customWidth="1"/>
+    <col min="12" max="12" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2402,8 +2417,14 @@
       <c r="O1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2447,7 +2468,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2491,7 +2512,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2532,7 +2553,7 @@
         <v>45297</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2576,7 +2597,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2620,7 +2641,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2658,7 +2679,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2699,7 +2720,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2743,7 +2764,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2784,7 +2805,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2828,7 +2849,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2869,7 +2890,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2934,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2954,7 +2975,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2998,7 +3019,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3039,7 +3060,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -3083,7 +3104,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -3124,7 +3145,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -3165,7 +3186,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -3209,7 +3230,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3250,7 +3271,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3294,7 +3315,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -3329,7 +3350,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -3364,7 +3385,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -3399,7 +3420,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3435,7 +3456,7 @@
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -3471,7 +3492,7 @@
       </c>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -3507,7 +3528,7 @@
       </c>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -3543,7 +3564,7 @@
       </c>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -3578,7 +3599,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3616,7 +3637,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3654,7 +3675,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -3689,7 +3710,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -3733,8 +3754,11 @@
       <c r="O34" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -3778,8 +3802,11 @@
       <c r="O35" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="8" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3849,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -3862,7 +3889,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -3907,7 +3934,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -3930,7 +3957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -3953,7 +3980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -3976,7 +4003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -3999,7 +4026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4022,7 +4049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4045,7 +4072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4068,7 +4095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4091,7 +4118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4114,7 +4141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -4137,7 +4164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4160,7 +4187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -4183,7 +4210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -4206,7 +4233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -4229,7 +4256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -4252,7 +4279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -4275,7 +4302,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -4298,7 +4325,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -4321,7 +4348,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -4344,7 +4371,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -4367,7 +4394,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -4390,7 +4417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -4413,7 +4440,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -4436,7 +4463,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -4459,7 +4486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -4482,7 +4509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -4505,7 +4532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -4528,7 +4555,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -4551,7 +4578,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -4574,7 +4601,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -4597,7 +4624,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -4620,7 +4647,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -4643,7 +4670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -4666,7 +4693,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -4689,7 +4716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -4712,7 +4739,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4735,7 +4762,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -4758,7 +4785,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -4781,7 +4808,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -4804,7 +4831,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -4827,7 +4854,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -4850,7 +4877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -4873,7 +4900,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -4896,7 +4923,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -4919,7 +4946,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -4942,7 +4969,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -4965,7 +4992,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -4988,7 +5015,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -5011,7 +5038,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -5034,7 +5061,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -5057,7 +5084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5080,7 +5107,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -5103,7 +5130,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -5126,7 +5153,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -5149,7 +5176,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -5172,7 +5199,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -5195,7 +5222,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -5218,7 +5245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -5241,7 +5268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -5264,7 +5291,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -5287,7 +5314,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -5310,7 +5337,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -5333,7 +5360,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -5356,7 +5383,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -5379,7 +5406,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -5402,7 +5429,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -5425,7 +5452,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -5448,7 +5475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -5471,7 +5498,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -5494,7 +5521,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -5517,7 +5544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -5540,7 +5567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -5563,7 +5590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -5586,7 +5613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -5609,7 +5636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -5632,7 +5659,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -5655,7 +5682,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -5678,7 +5705,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -5701,7 +5728,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -5724,7 +5751,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -5747,7 +5774,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -5770,7 +5797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -5793,7 +5820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -5816,7 +5843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -5839,7 +5866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -5862,7 +5889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -5885,7 +5912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -5908,7 +5935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -5931,7 +5958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -5954,7 +5981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -5977,7 +6004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -6000,7 +6027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -6023,7 +6050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -6046,7 +6073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -6069,7 +6096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -6092,7 +6119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -6115,7 +6142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -6138,7 +6165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -6161,7 +6188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -6184,7 +6211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -6207,7 +6234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -6230,7 +6257,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -6253,7 +6280,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -6276,7 +6303,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -6299,7 +6326,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -6322,7 +6349,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -6345,7 +6372,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -6368,7 +6395,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -6391,7 +6418,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>7</v>
       </c>
@@ -6414,7 +6441,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -6437,7 +6464,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -6460,7 +6487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -6483,7 +6510,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -6506,7 +6533,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -6529,7 +6556,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -6552,7 +6579,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>7</v>
       </c>
@@ -6575,7 +6602,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -6598,7 +6625,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -6621,7 +6648,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>7</v>
       </c>
@@ -6644,7 +6671,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -6667,7 +6694,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -6690,7 +6717,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>7</v>
       </c>
@@ -6713,7 +6740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -6736,7 +6763,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>7</v>
       </c>
@@ -6759,7 +6786,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>7</v>
       </c>
@@ -6782,7 +6809,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>7</v>
       </c>
@@ -6805,7 +6832,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -6828,7 +6855,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>7</v>
       </c>
@@ -6851,7 +6878,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>7</v>
       </c>
@@ -6874,7 +6901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -6897,7 +6924,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -6920,7 +6947,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -6943,7 +6970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>7</v>
       </c>
@@ -6966,7 +6993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -6989,7 +7016,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>7</v>
       </c>
@@ -7012,7 +7039,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>7</v>
       </c>
@@ -7035,7 +7062,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>7</v>
       </c>
@@ -7058,7 +7085,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>7</v>
       </c>
@@ -7081,7 +7108,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -7104,7 +7131,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>7</v>
       </c>
@@ -7127,7 +7154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>7</v>
       </c>
@@ -7150,7 +7177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>7</v>
       </c>
@@ -7173,7 +7200,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -7196,7 +7223,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -7219,7 +7246,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -7242,7 +7269,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -7265,7 +7292,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -7288,7 +7315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -7311,7 +7338,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -7334,7 +7361,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -7357,7 +7384,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -7380,7 +7407,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>7</v>
       </c>
@@ -7403,7 +7430,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -7426,7 +7453,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -7449,7 +7476,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -7472,7 +7499,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -7495,7 +7522,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -7518,7 +7545,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -7541,7 +7568,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -7564,7 +7591,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -7587,7 +7614,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -7610,7 +7637,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>7</v>
       </c>
@@ -7633,7 +7660,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -7656,7 +7683,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>7</v>
       </c>
@@ -7679,7 +7706,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -7702,7 +7729,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>7</v>
       </c>
@@ -7725,7 +7752,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>7</v>
       </c>
@@ -7748,7 +7775,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>7</v>
       </c>
@@ -7771,7 +7798,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>7</v>
       </c>
@@ -7794,7 +7821,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>7</v>
       </c>
@@ -7817,7 +7844,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>7</v>
       </c>
@@ -7840,7 +7867,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="210" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -7863,7 +7890,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>7</v>
       </c>
@@ -7886,7 +7913,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -7909,7 +7936,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="213" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>7</v>
       </c>
@@ -7932,7 +7959,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>7</v>
       </c>
@@ -7955,7 +7982,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>7</v>
       </c>
@@ -7978,7 +8005,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>7</v>
       </c>
@@ -8001,7 +8028,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -8024,7 +8051,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -8047,7 +8074,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>7</v>
       </c>
@@ -8070,7 +8097,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>7</v>
       </c>
@@ -8093,7 +8120,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>7</v>
       </c>
@@ -8116,7 +8143,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -8161,7 +8188,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="223" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -8202,7 +8229,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -8247,7 +8274,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -8291,7 +8318,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -8369,19 +8396,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD7F955-AF0A-4814-8374-5E8081EA0170}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>602</v>
       </c>
@@ -8398,7 +8425,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>605</v>
       </c>
@@ -8409,7 +8436,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>606</v>
       </c>
@@ -8423,7 +8450,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>607</v>
       </c>
@@ -8440,7 +8467,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>607</v>
       </c>
@@ -8454,7 +8481,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>607</v>
       </c>
@@ -8468,7 +8495,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>607</v>
       </c>
@@ -8482,7 +8509,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>608</v>
       </c>
@@ -8496,7 +8523,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>608</v>
       </c>
@@ -8507,7 +8534,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>608</v>
       </c>
@@ -8518,7 +8545,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>609</v>
       </c>
@@ -8529,7 +8556,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>609</v>
       </c>
@@ -8543,7 +8570,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>609</v>
       </c>
@@ -8557,7 +8584,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>609</v>
       </c>
@@ -8571,7 +8598,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>609</v>
       </c>
@@ -8585,7 +8612,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>609</v>
       </c>
@@ -8599,7 +8626,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>609</v>
       </c>
@@ -8610,7 +8637,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>609</v>
       </c>

</xml_diff>

<commit_message>
changes on the ay to austria
</commit_message>
<xml_diff>
--- a/admin/IB_OB_FLD.xlsx
+++ b/admin/IB_OB_FLD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RW\EAISI-Pythia\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C193D-FC77-4E4D-AAF2-9A88F1C48693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089076E3-C333-43EB-8108-67AF1D56698E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-110" windowWidth="37430" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_LOADS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="624">
   <si>
     <t>SYSTID</t>
   </si>
@@ -1882,13 +1882,76 @@
   max( /BIC/ASDSFRPR17~/BIC/VERSMON )
  FROM 
   /BIC/ASDSFRPR17</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>1. DTP select current Month for VERSMON, e.g. 2025xx
+2. extract
+3. AL11 SDSFRPR1.csv
+4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRLV1_2025xx.csv</t>
+  </si>
+  <si>
+    <t>1. DTP select current Month for VERSMON M-1 for CALMONTH, e.g. 2025xx
+2. extract
+3. AL11 SDSFRPR1.csv
+4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRPR1_20250X.csv</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>1. DTP select current Month for VERSMON, e.g. 2025xx
+2. extract
+3. AL11 SDSFRPR3.csv
+4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRLV3_2025xx.csv</t>
+  </si>
+  <si>
+    <t>1. DTP select current Month for VERSMON, e.g. 2025xx
+2. extract
+3. AL11 SDSFRPR2.csv
+4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRPR2_20250X.csv</t>
+  </si>
+  <si>
+    <t>✔202502</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0. POSTDR FORECAST MADE THIS MONTH (end of the month)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. DTP select current Month for VERSMON, e.g. 2025xx
+2. extract
+3. AL11 SDSFRPR4.csv
+4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRPR4_20250X.csv</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1922,6 +1985,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2006,8 +2077,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:Q226" totalsRowShown="0">
-  <autoFilter ref="A1:Q226" xr:uid="{00000000-0009-0000-0100-000003000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:R226" totalsRowShown="0">
+  <autoFilter ref="A1:R226" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="8">
       <filters>
         <filter val="OH_FRPR1"/>
@@ -2016,23 +2087,16 @@
         <filter val="OH_FRPR4"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="11">
+    <filterColumn colId="15">
       <filters>
-        <filter val="SDSFRLV1_202412_2021"/>
-        <filter val="SDSFRLV1_202501"/>
-        <filter val="SDSFRLV3_202412_2021"/>
-        <filter val="SDSFRLV3_202501"/>
-        <filter val="SDSFRPR1_2024XX"/>
-        <filter val="SDSFRPR1_20250X"/>
-        <filter val="SDSFRPR3_2024XX"/>
-        <filter val="SDSFRPR3_20250X"/>
+        <filter val="YES"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:O226">
     <sortCondition ref="L34:L226"/>
   </sortState>
-  <tableColumns count="17">
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SYSTID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CLIENT"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FILEINTERN"/>
@@ -2050,6 +2114,7 @@
     <tableColumn id="18" xr3:uid="{F55B9E97-2B13-448C-B575-C4B0834B5962}" name="Column1"/>
     <tableColumn id="12" xr3:uid="{1CB3EDD4-A8FA-46CF-AA4F-81B2540CF816}" name="REPEAT"/>
     <tableColumn id="13" xr3:uid="{03A11749-D3F7-4D01-A89C-2C1F0AB0E80A}" name="SQL"/>
+    <tableColumn id="15" xr3:uid="{3BDB626A-EE52-4078-9820-62AA5A68BF01}" name="Procedure"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2348,30 +2413,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q226"/>
+  <dimension ref="A1:R226"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L232" sqref="L232"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="R231" sqref="R231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" customWidth="1"/>
-    <col min="8" max="8" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.08984375" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" customWidth="1"/>
-    <col min="12" max="12" width="35.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="45.81640625" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="5.21875" customWidth="1"/>
+    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.77734375" customWidth="1"/>
+    <col min="18" max="18" width="97.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2423,8 +2489,11 @@
       <c r="Q1" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2468,7 +2537,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2512,7 +2581,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2553,7 +2622,7 @@
         <v>45297</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2597,7 +2666,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2641,7 +2710,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2679,7 +2748,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2720,7 +2789,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2764,7 +2833,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2805,7 +2874,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2849,7 +2918,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2890,7 +2959,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2934,7 +3003,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2975,7 +3044,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -3019,7 +3088,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3060,7 +3129,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -3104,7 +3173,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -3145,7 +3214,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -3186,7 +3255,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -3230,7 +3299,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3271,7 +3340,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3384,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -3350,7 +3419,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -3385,7 +3454,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -3420,7 +3489,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3456,7 +3525,7 @@
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -3492,7 +3561,7 @@
       </c>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -3528,7 +3597,7 @@
       </c>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -3564,7 +3633,7 @@
       </c>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -3599,7 +3668,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3637,7 +3706,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3675,7 +3744,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -3710,7 +3779,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -3757,8 +3826,11 @@
       <c r="P34" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R34" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -3796,17 +3868,23 @@
         <v>566</v>
       </c>
       <c r="M35" s="2">
-        <v>45676</v>
+        <v>45698</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" t="s">
         <v>562</v>
       </c>
+      <c r="P35" t="s">
+        <v>619</v>
+      </c>
       <c r="Q35" s="8" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R35" s="8" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -3843,13 +3921,21 @@
       <c r="L36" t="s">
         <v>559</v>
       </c>
-      <c r="M36" s="2"/>
+      <c r="M36" s="2">
+        <v>45698</v>
+      </c>
       <c r="N36" s="4"/>
       <c r="O36" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P36" t="s">
+        <v>619</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -3871,7 +3957,7 @@
       <c r="G37" t="s">
         <v>394</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="3" t="s">
         <v>552</v>
       </c>
       <c r="I37" t="s">
@@ -3886,10 +3972,21 @@
       <c r="L37" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="M37" s="2"/>
+      <c r="M37" s="2">
+        <v>45698</v>
+      </c>
       <c r="N37" s="4"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="O37" t="s">
+        <v>622</v>
+      </c>
+      <c r="P37" t="s">
+        <v>619</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -3933,8 +4030,14 @@
       <c r="O38" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P38" t="s">
+        <v>612</v>
+      </c>
+      <c r="R38" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -3957,7 +4060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -3980,7 +4083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4003,7 +4106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4026,7 +4129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4049,7 +4152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4072,7 +4175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4095,7 +4198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4141,7 +4244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -4164,7 +4267,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4187,7 +4290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -4210,7 +4313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -4233,7 +4336,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -4256,7 +4359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -4279,7 +4382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -4302,7 +4405,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -4325,7 +4428,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -4348,7 +4451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -4371,7 +4474,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -4394,7 +4497,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -4417,7 +4520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -4440,7 +4543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -4463,7 +4566,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -4486,7 +4589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -4509,7 +4612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -4532,7 +4635,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -4555,7 +4658,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -4578,7 +4681,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -4601,7 +4704,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4727,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -4647,7 +4750,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -4670,7 +4773,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -4693,7 +4796,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -4716,7 +4819,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -4739,7 +4842,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4762,7 +4865,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -4785,7 +4888,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -4808,7 +4911,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -4831,7 +4934,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -4854,7 +4957,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -4877,7 +4980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -4900,7 +5003,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -4923,7 +5026,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -4946,7 +5049,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -4969,7 +5072,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +5095,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -5015,7 +5118,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -5038,7 +5141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -5061,7 +5164,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -5084,7 +5187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5107,7 +5210,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -5130,7 +5233,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -5153,7 +5256,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -5176,7 +5279,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -5199,7 +5302,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -5222,7 +5325,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -5245,7 +5348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -5268,7 +5371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -5291,7 +5394,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -5314,7 +5417,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -5337,7 +5440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -5360,7 +5463,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -5383,7 +5486,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -5406,7 +5509,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -5429,7 +5532,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -5452,7 +5555,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -5475,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -5498,7 +5601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -5521,7 +5624,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -5544,7 +5647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -5567,7 +5670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -5590,7 +5693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -5613,7 +5716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -5636,7 +5739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -5659,7 +5762,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -5682,7 +5785,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -5705,7 +5808,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -5728,7 +5831,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -5751,7 +5854,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -5774,7 +5877,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -5797,7 +5900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -5820,7 +5923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -5843,7 +5946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -5866,7 +5969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -5889,7 +5992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -5912,7 +6015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -5935,7 +6038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -5958,7 +6061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -5981,7 +6084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -6004,7 +6107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -6027,7 +6130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -6050,7 +6153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -6073,7 +6176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -6096,7 +6199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -6119,7 +6222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -6142,7 +6245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -6165,7 +6268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -6188,7 +6291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -6211,7 +6314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -6234,7 +6337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -6257,7 +6360,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -6280,7 +6383,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -6303,7 +6406,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -6326,7 +6429,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -6349,7 +6452,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -6372,7 +6475,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -6395,7 +6498,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -6418,7 +6521,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>7</v>
       </c>
@@ -6441,7 +6544,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -6464,7 +6567,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -6487,7 +6590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -6510,7 +6613,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -6533,7 +6636,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -6556,7 +6659,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -6579,7 +6682,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>7</v>
       </c>
@@ -6602,7 +6705,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -6625,7 +6728,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -6648,7 +6751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>7</v>
       </c>
@@ -6671,7 +6774,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -6694,7 +6797,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -6717,7 +6820,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>7</v>
       </c>
@@ -6740,7 +6843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -6763,7 +6866,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>7</v>
       </c>
@@ -6786,7 +6889,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>7</v>
       </c>
@@ -6809,7 +6912,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>7</v>
       </c>
@@ -6832,7 +6935,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -6855,7 +6958,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>7</v>
       </c>
@@ -6878,7 +6981,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>7</v>
       </c>
@@ -6901,7 +7004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -6924,7 +7027,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -6947,7 +7050,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -6970,7 +7073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>7</v>
       </c>
@@ -6993,7 +7096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -7016,7 +7119,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>7</v>
       </c>
@@ -7039,7 +7142,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>7</v>
       </c>
@@ -7062,7 +7165,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>7</v>
       </c>
@@ -7085,7 +7188,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>7</v>
       </c>
@@ -7108,7 +7211,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -7131,7 +7234,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>7</v>
       </c>
@@ -7154,7 +7257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>7</v>
       </c>
@@ -7177,7 +7280,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>7</v>
       </c>
@@ -7200,7 +7303,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -7223,7 +7326,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -7246,7 +7349,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -7269,7 +7372,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -7292,7 +7395,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -7315,7 +7418,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -7338,7 +7441,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -7361,7 +7464,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -7384,7 +7487,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -7407,7 +7510,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>7</v>
       </c>
@@ -7430,7 +7533,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -7453,7 +7556,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -7476,7 +7579,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -7499,7 +7602,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -7522,7 +7625,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -7545,7 +7648,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -7568,7 +7671,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -7591,7 +7694,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -7614,7 +7717,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -7637,7 +7740,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>7</v>
       </c>
@@ -7660,7 +7763,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -7683,7 +7786,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>7</v>
       </c>
@@ -7706,7 +7809,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -7729,7 +7832,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>7</v>
       </c>
@@ -7752,7 +7855,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>7</v>
       </c>
@@ -7775,7 +7878,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>7</v>
       </c>
@@ -7798,7 +7901,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>7</v>
       </c>
@@ -7821,7 +7924,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>7</v>
       </c>
@@ -7844,7 +7947,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>7</v>
       </c>
@@ -7867,7 +7970,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="210" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -7890,7 +7993,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>7</v>
       </c>
@@ -7913,7 +8016,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -7936,7 +8039,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="213" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>7</v>
       </c>
@@ -7959,7 +8062,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>7</v>
       </c>
@@ -7982,7 +8085,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>7</v>
       </c>
@@ -8005,7 +8108,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="216" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>7</v>
       </c>
@@ -8028,7 +8131,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -8051,7 +8154,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -8074,7 +8177,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>7</v>
       </c>
@@ -8097,7 +8200,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>7</v>
       </c>
@@ -8120,7 +8223,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>7</v>
       </c>
@@ -8143,7 +8246,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:18" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -8187,8 +8290,14 @@
       <c r="O222" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P222" t="s">
+        <v>612</v>
+      </c>
+      <c r="R222" s="8" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -8228,8 +8337,11 @@
       <c r="O223" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P223" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -8273,8 +8385,11 @@
       <c r="O224" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P224" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -8296,7 +8411,7 @@
       <c r="G225" t="s">
         <v>394</v>
       </c>
-      <c r="H225" t="s">
+      <c r="H225" s="3" t="s">
         <v>491</v>
       </c>
       <c r="I225" t="s">
@@ -8312,13 +8427,22 @@
         <v>530</v>
       </c>
       <c r="M225" s="2">
-        <v>45301</v>
+        <v>45698</v>
       </c>
       <c r="N225" s="4" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O225" t="s">
+        <v>622</v>
+      </c>
+      <c r="P225" t="s">
+        <v>619</v>
+      </c>
+      <c r="R225" s="8" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -8361,6 +8485,9 @@
       <c r="N226" s="4"/>
       <c r="O226" t="s">
         <v>563</v>
+      </c>
+      <c r="P226" t="s">
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -8380,14 +8507,16 @@
     <hyperlink ref="H223" r:id="rId13" xr:uid="{41332EAD-A7D8-4B98-9AEA-B3C46DB09FE5}"/>
     <hyperlink ref="H34" r:id="rId14" xr:uid="{79082468-4277-4D99-964E-5A90DAA08494}"/>
     <hyperlink ref="H38" r:id="rId15" xr:uid="{BA35A75B-7054-45CE-8912-3BA4D8B39C31}"/>
+    <hyperlink ref="H37" r:id="rId16" xr:uid="{9C9BD80B-F08F-40DF-825D-DFE6F8944C50}"/>
+    <hyperlink ref="H225" r:id="rId17" xr:uid="{D11407FF-FDDA-44CC-ACB4-55BACEA0299A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId17"/>
+    <customPr name="_pios_id" r:id="rId19"/>
   </customProperties>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8400,15 +8529,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>602</v>
       </c>
@@ -8425,7 +8554,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>605</v>
       </c>
@@ -8436,7 +8565,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>606</v>
       </c>
@@ -8450,7 +8579,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>607</v>
       </c>
@@ -8467,7 +8596,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>607</v>
       </c>
@@ -8481,7 +8610,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>607</v>
       </c>
@@ -8495,7 +8624,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>607</v>
       </c>
@@ -8509,7 +8638,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>608</v>
       </c>
@@ -8523,7 +8652,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>608</v>
       </c>
@@ -8534,7 +8663,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>608</v>
       </c>
@@ -8545,7 +8674,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>609</v>
       </c>
@@ -8556,7 +8685,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>609</v>
       </c>
@@ -8570,7 +8699,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>609</v>
       </c>
@@ -8584,7 +8713,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>609</v>
       </c>
@@ -8598,7 +8727,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>609</v>
       </c>
@@ -8612,7 +8741,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>609</v>
       </c>
@@ -8626,7 +8755,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>609</v>
       </c>
@@ -8637,7 +8766,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>609</v>
       </c>
@@ -8653,8 +8782,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId1"/>
+  </customProperties>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update from ecotone pc
</commit_message>
<xml_diff>
--- a/admin/IB_OB_FLD.xlsx
+++ b/admin/IB_OB_FLD.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RW\EAISI-Pythia\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089076E3-C333-43EB-8108-67AF1D56698E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472FAA34-076D-43F8-A257-448E73A96050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="-110" windowWidth="37190" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_LOADS" sheetId="1" r:id="rId1"/>
-    <sheet name="PATHS" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="PATHS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentManualCount="8"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="625">
   <si>
     <t>SYSTID</t>
   </si>
@@ -1945,6 +1946,9 @@
 3. AL11 SDSFRPR4.csv
 4. Move to folder C:\PW\OneDrive\ET\pythia\data\production\Bronze\sales\SDSFRPR4_20250X.csv</t>
     </r>
+  </si>
+  <si>
+    <t>bwmt://WTB/sap/bw/modeling/dtpa/dtp_006eipubipunxgfylzhb6f3gv/m</t>
   </si>
 </sst>
 </file>
@@ -2415,29 +2419,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R226"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="119" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="119" workbookViewId="0">
       <selection activeCell="R231" sqref="R231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" customWidth="1"/>
+    <col min="8" max="8" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="45.77734375" customWidth="1"/>
-    <col min="18" max="18" width="97.77734375" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" customWidth="1"/>
+    <col min="12" max="12" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.81640625" customWidth="1"/>
+    <col min="18" max="18" width="97.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +2497,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2541,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2581,7 +2585,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2622,7 +2626,7 @@
         <v>45297</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2666,7 +2670,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2748,7 +2752,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2833,7 +2837,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -3003,7 +3007,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3044,7 +3048,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -3088,7 +3092,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3129,7 +3133,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -3173,7 +3177,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -3255,7 +3259,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3384,7 +3388,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -3419,7 +3423,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -3489,7 +3493,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3525,7 +3529,7 @@
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -3561,7 +3565,7 @@
       </c>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -3597,7 +3601,7 @@
       </c>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -3633,7 +3637,7 @@
       </c>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -3668,7 +3672,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3706,7 +3710,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3744,7 +3748,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -3779,7 +3783,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -3830,7 +3834,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -3884,7 +3888,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -3935,7 +3939,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -3986,7 +3990,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4037,7 +4041,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4060,7 +4064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4129,7 +4133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4152,7 +4156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4175,7 +4179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4198,7 +4202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4221,7 +4225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4244,7 +4248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -4267,7 +4271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4290,7 +4294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -4313,7 +4317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -4336,7 +4340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -4359,7 +4363,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -4382,7 +4386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -4405,7 +4409,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -4428,7 +4432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -4451,7 +4455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -4474,7 +4478,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -4497,7 +4501,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -4520,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -4543,7 +4547,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -4566,7 +4570,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -4589,7 +4593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -4612,7 +4616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -4658,7 +4662,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -4681,7 +4685,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -4704,7 +4708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -4727,7 +4731,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -4750,7 +4754,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -4773,7 +4777,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -4796,7 +4800,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -4819,7 +4823,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -4842,7 +4846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4865,7 +4869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -4888,7 +4892,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -4911,7 +4915,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -4934,7 +4938,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -4957,7 +4961,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -4980,7 +4984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -5003,7 +5007,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -5026,7 +5030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -5049,7 +5053,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -5072,7 +5076,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -5095,7 +5099,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -5118,7 +5122,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -5141,7 +5145,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -5164,7 +5168,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -5187,7 +5191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5210,7 +5214,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -5233,7 +5237,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -5256,7 +5260,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -5279,7 +5283,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -5325,7 +5329,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -5348,7 +5352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -5371,7 +5375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -5394,7 +5398,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -5417,7 +5421,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -5440,7 +5444,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -5463,7 +5467,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -5486,7 +5490,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -5509,7 +5513,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -5532,7 +5536,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -5555,7 +5559,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -5578,7 +5582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -5601,7 +5605,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -5624,7 +5628,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -5647,7 +5651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -5670,7 +5674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -5693,7 +5697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -5716,7 +5720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -5739,7 +5743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -5762,7 +5766,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>7</v>
       </c>
@@ -5785,7 +5789,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -5808,7 +5812,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -5831,7 +5835,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -5854,7 +5858,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -5877,7 +5881,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>7</v>
       </c>
@@ -5900,7 +5904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -5923,7 +5927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -5946,7 +5950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -5969,7 +5973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -5992,7 +5996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -6015,7 +6019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -6038,7 +6042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -6061,7 +6065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -6084,7 +6088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -6107,7 +6111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -6130,7 +6134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -6153,7 +6157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -6176,7 +6180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -6199,7 +6203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -6222,7 +6226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -6245,7 +6249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -6268,7 +6272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -6291,7 +6295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -6314,7 +6318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -6337,7 +6341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>7</v>
       </c>
@@ -6360,7 +6364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -6383,7 +6387,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -6406,7 +6410,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -6429,7 +6433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -6452,7 +6456,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -6475,7 +6479,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -6498,7 +6502,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -6521,7 +6525,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>7</v>
       </c>
@@ -6544,7 +6548,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -6567,7 +6571,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -6590,7 +6594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -6613,7 +6617,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -6636,7 +6640,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -6659,7 +6663,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -6682,7 +6686,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>7</v>
       </c>
@@ -6705,7 +6709,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -6728,7 +6732,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -6751,7 +6755,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>7</v>
       </c>
@@ -6774,7 +6778,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -6797,7 +6801,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -6820,7 +6824,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>7</v>
       </c>
@@ -6843,7 +6847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -6866,7 +6870,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>7</v>
       </c>
@@ -6889,7 +6893,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>7</v>
       </c>
@@ -6912,7 +6916,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>7</v>
       </c>
@@ -6935,7 +6939,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -6958,7 +6962,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>7</v>
       </c>
@@ -6981,7 +6985,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>7</v>
       </c>
@@ -7004,7 +7008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -7027,7 +7031,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -7050,7 +7054,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -7073,7 +7077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>7</v>
       </c>
@@ -7096,7 +7100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -7119,7 +7123,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>7</v>
       </c>
@@ -7142,7 +7146,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>7</v>
       </c>
@@ -7165,7 +7169,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>7</v>
       </c>
@@ -7188,7 +7192,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>7</v>
       </c>
@@ -7211,7 +7215,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>7</v>
       </c>
@@ -7257,7 +7261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>7</v>
       </c>
@@ -7280,7 +7284,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>7</v>
       </c>
@@ -7303,7 +7307,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -7326,7 +7330,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -7349,7 +7353,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>7</v>
       </c>
@@ -7372,7 +7376,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -7395,7 +7399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -7418,7 +7422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>7</v>
       </c>
@@ -7441,7 +7445,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -7464,7 +7468,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -7487,7 +7491,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -7510,7 +7514,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>7</v>
       </c>
@@ -7533,7 +7537,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -7556,7 +7560,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>7</v>
       </c>
@@ -7579,7 +7583,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -7602,7 +7606,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -7625,7 +7629,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>7</v>
       </c>
@@ -7648,7 +7652,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>7</v>
       </c>
@@ -7671,7 +7675,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -7694,7 +7698,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -7717,7 +7721,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>7</v>
       </c>
@@ -7740,7 +7744,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>7</v>
       </c>
@@ -7763,7 +7767,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -7786,7 +7790,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>7</v>
       </c>
@@ -7809,7 +7813,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -7832,7 +7836,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>7</v>
       </c>
@@ -7855,7 +7859,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>7</v>
       </c>
@@ -7878,7 +7882,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>7</v>
       </c>
@@ -7901,7 +7905,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>7</v>
       </c>
@@ -7924,7 +7928,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>7</v>
       </c>
@@ -7947,7 +7951,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>7</v>
       </c>
@@ -7970,7 +7974,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -7993,7 +7997,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>7</v>
       </c>
@@ -8016,7 +8020,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -8039,7 +8043,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>7</v>
       </c>
@@ -8062,7 +8066,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>7</v>
       </c>
@@ -8085,7 +8089,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>7</v>
       </c>
@@ -8108,7 +8112,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>7</v>
       </c>
@@ -8131,7 +8135,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -8154,7 +8158,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -8177,7 +8181,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>7</v>
       </c>
@@ -8200,7 +8204,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>7</v>
       </c>
@@ -8223,7 +8227,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>7</v>
       </c>
@@ -8246,7 +8250,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>7</v>
       </c>
@@ -8297,7 +8301,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>7</v>
       </c>
@@ -8341,7 +8345,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -8389,7 +8393,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="225" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -8442,7 +8446,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -8522,6 +8526,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A980CAAD-CF82-485F-B31B-6543207747EB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>624</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{6DEC0F40-69A6-47A6-8790-B14A5C8F76B2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD7F955-AF0A-4814-8374-5E8081EA0170}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -8529,15 +8559,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>602</v>
       </c>
@@ -8554,7 +8584,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>605</v>
       </c>
@@ -8565,7 +8595,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>606</v>
       </c>
@@ -8579,7 +8609,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>607</v>
       </c>
@@ -8596,7 +8626,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>607</v>
       </c>
@@ -8610,7 +8640,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>607</v>
       </c>
@@ -8624,7 +8654,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>607</v>
       </c>
@@ -8638,7 +8668,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>608</v>
       </c>
@@ -8652,7 +8682,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>608</v>
       </c>
@@ -8663,7 +8693,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>608</v>
       </c>
@@ -8674,7 +8704,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>609</v>
       </c>
@@ -8685,7 +8715,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>609</v>
       </c>
@@ -8699,7 +8729,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>609</v>
       </c>
@@ -8713,7 +8743,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>609</v>
       </c>
@@ -8727,7 +8757,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>609</v>
       </c>
@@ -8741,7 +8771,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>609</v>
       </c>
@@ -8755,7 +8785,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>609</v>
       </c>
@@ -8766,7 +8796,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>609</v>
       </c>

</xml_diff>

<commit_message>
xlsx with new DTP
</commit_message>
<xml_diff>
--- a/admin/IB_OB_FLD.xlsx
+++ b/admin/IB_OB_FLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RW\EAISI-Pythia\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634E1197-965E-4778-B296-2592143037A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F657AA0-B77D-47F0-BED9-37FE06B2D5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="-110" windowWidth="37190" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DATA_LOADS" sheetId="1" r:id="rId1"/>
     <sheet name="PATHS" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029" concurrentManualCount="14"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="629">
   <si>
     <t>SYSTID</t>
   </si>
@@ -1953,13 +1953,13 @@
     <t>DD_SALES_QTY_2023</t>
   </si>
   <si>
-    <t>DTP_006EIZGR39XAWQANS1LNUZF2Y</t>
-  </si>
-  <si>
-    <t>DTP_006EIZGR39XAWQANYOZZI4HSQ</t>
-  </si>
-  <si>
     <t>DTP_006EICO68TUM2BI6L8H246CK6</t>
+  </si>
+  <si>
+    <t>DTP_006EICO68TVC45HDCJLST83KQ</t>
+  </si>
+  <si>
+    <t>DTP_006EICO68TVC45HDHUE4L6TQY</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2046,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2062,6 +2062,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2416,8 +2417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R229"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2646,7 +2647,7 @@
         <v>394</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="I5" t="s">
         <v>463</v>
@@ -2663,6 +2664,9 @@
       <c r="M5" s="2">
         <v>45825</v>
       </c>
+      <c r="N5" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="P5" t="s">
         <v>611</v>
       </c>
@@ -2690,7 +2694,7 @@
         <v>394</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="I6" t="s">
         <v>463</v>
@@ -2707,6 +2711,9 @@
       <c r="M6" s="2">
         <v>45825</v>
       </c>
+      <c r="N6" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="P6" t="s">
         <v>611</v>
       </c>
@@ -2734,7 +2741,7 @@
         <v>394</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="I7" t="s">
         <v>463</v>
@@ -2792,7 +2799,7 @@
       <c r="K8" t="s">
         <v>538</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="9" t="s">
         <v>546</v>
       </c>
       <c r="M8" s="2">
@@ -2839,7 +2846,7 @@
       <c r="K9" t="s">
         <v>538</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="9" t="s">
         <v>547</v>
       </c>
       <c r="M9" s="2">
@@ -8634,36 +8641,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L8" r:id="rId1" xr:uid="{60F239C9-7000-4310-B526-00F9A909BB8F}"/>
-    <hyperlink ref="L9" r:id="rId2" xr:uid="{09C5F614-FEA5-4BE6-9AF4-B58DB17E1928}"/>
-    <hyperlink ref="L14" r:id="rId3" location="BWProcessChain-change?chainId=LC_DYN_PERKZ_W" xr:uid="{C1C40E84-A93D-462B-B319-3E48BD1A540C}"/>
-    <hyperlink ref="L2" r:id="rId4" xr:uid="{B815E112-DF4A-4A6A-A208-89D4A68B3073}"/>
-    <hyperlink ref="L40" r:id="rId5" xr:uid="{5F8E6099-3933-4328-A7B9-6AADD4120355}"/>
-    <hyperlink ref="L228" r:id="rId6" xr:uid="{0A889FA1-F3A2-4F5E-A6DB-7EFD384A1B18}"/>
-    <hyperlink ref="L3" r:id="rId7" xr:uid="{98AA934F-9CE8-4A25-88E5-A2AE5ECA8184}"/>
-    <hyperlink ref="H227" r:id="rId8" xr:uid="{91DB4B05-B319-4BAE-9536-832A996B0A93}"/>
-    <hyperlink ref="H39" r:id="rId9" xr:uid="{B69C832F-9AED-4383-BEAE-88891483874D}"/>
-    <hyperlink ref="H38" r:id="rId10" xr:uid="{5168AB38-C1A4-4BD6-B77F-65D4F0E10F24}"/>
-    <hyperlink ref="H229" r:id="rId11" xr:uid="{AEDB3E06-2740-4324-9CEB-961490958D39}"/>
-    <hyperlink ref="H225" r:id="rId12" xr:uid="{40520CCD-1EAC-4359-8806-34234068BCB5}"/>
-    <hyperlink ref="H226" r:id="rId13" xr:uid="{41332EAD-A7D8-4B98-9AEA-B3C46DB09FE5}"/>
-    <hyperlink ref="H37" r:id="rId14" xr:uid="{79082468-4277-4D99-964E-5A90DAA08494}"/>
-    <hyperlink ref="H41" r:id="rId15" xr:uid="{BA35A75B-7054-45CE-8912-3BA4D8B39C31}"/>
-    <hyperlink ref="H40" r:id="rId16" xr:uid="{9C9BD80B-F08F-40DF-825D-DFE6F8944C50}"/>
-    <hyperlink ref="H228" r:id="rId17" xr:uid="{D11407FF-FDDA-44CC-ACB4-55BACEA0299A}"/>
-    <hyperlink ref="H8" r:id="rId18" xr:uid="{6F3F9826-38F4-42E7-A0B5-0FF7DE8B50D7}"/>
-    <hyperlink ref="H9" r:id="rId19" xr:uid="{2D5FB69D-2D58-4858-BE91-169CC59504A3}"/>
-    <hyperlink ref="H7" r:id="rId20" xr:uid="{B5DA7ABF-824A-4D10-A69E-FA04FBAF5468}"/>
-    <hyperlink ref="H6" r:id="rId21" xr:uid="{CCF15709-7CA0-45F4-AE32-B95BCA2149A6}"/>
-    <hyperlink ref="H5" r:id="rId22" xr:uid="{869A39E9-CC15-43F2-B4B0-115C939D74C7}"/>
+    <hyperlink ref="L14" r:id="rId1" location="BWProcessChain-change?chainId=LC_DYN_PERKZ_W" xr:uid="{C1C40E84-A93D-462B-B319-3E48BD1A540C}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{B815E112-DF4A-4A6A-A208-89D4A68B3073}"/>
+    <hyperlink ref="L40" r:id="rId3" xr:uid="{5F8E6099-3933-4328-A7B9-6AADD4120355}"/>
+    <hyperlink ref="L228" r:id="rId4" xr:uid="{0A889FA1-F3A2-4F5E-A6DB-7EFD384A1B18}"/>
+    <hyperlink ref="L3" r:id="rId5" xr:uid="{98AA934F-9CE8-4A25-88E5-A2AE5ECA8184}"/>
+    <hyperlink ref="H227" r:id="rId6" xr:uid="{91DB4B05-B319-4BAE-9536-832A996B0A93}"/>
+    <hyperlink ref="H39" r:id="rId7" xr:uid="{B69C832F-9AED-4383-BEAE-88891483874D}"/>
+    <hyperlink ref="H38" r:id="rId8" xr:uid="{5168AB38-C1A4-4BD6-B77F-65D4F0E10F24}"/>
+    <hyperlink ref="H229" r:id="rId9" xr:uid="{AEDB3E06-2740-4324-9CEB-961490958D39}"/>
+    <hyperlink ref="H225" r:id="rId10" xr:uid="{40520CCD-1EAC-4359-8806-34234068BCB5}"/>
+    <hyperlink ref="H226" r:id="rId11" xr:uid="{41332EAD-A7D8-4B98-9AEA-B3C46DB09FE5}"/>
+    <hyperlink ref="H37" r:id="rId12" xr:uid="{79082468-4277-4D99-964E-5A90DAA08494}"/>
+    <hyperlink ref="H41" r:id="rId13" xr:uid="{BA35A75B-7054-45CE-8912-3BA4D8B39C31}"/>
+    <hyperlink ref="H40" r:id="rId14" xr:uid="{9C9BD80B-F08F-40DF-825D-DFE6F8944C50}"/>
+    <hyperlink ref="H228" r:id="rId15" xr:uid="{D11407FF-FDDA-44CC-ACB4-55BACEA0299A}"/>
+    <hyperlink ref="H8" r:id="rId16" xr:uid="{6F3F9826-38F4-42E7-A0B5-0FF7DE8B50D7}"/>
+    <hyperlink ref="H9" r:id="rId17" xr:uid="{2D5FB69D-2D58-4858-BE91-169CC59504A3}"/>
+    <hyperlink ref="H7" r:id="rId18" xr:uid="{B5DA7ABF-824A-4D10-A69E-FA04FBAF5468}"/>
+    <hyperlink ref="H5" r:id="rId19" xr:uid="{0C6D7D18-0D11-4A86-949E-9A7F0B9515C4}"/>
+    <hyperlink ref="H6" r:id="rId20" xr:uid="{7F2C903F-F7B3-4A1A-95F9-E78F395A47E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId24"/>
+    <customPr name="_pios_id" r:id="rId22"/>
   </customProperties>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>